<commit_message>
Projeto v0.9 Criado executavel para testes
</commit_message>
<xml_diff>
--- a/ExemploContatosEnviar.xlsx
+++ b/ExemploContatosEnviar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20343"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D18_20\Desktop\EnviarWhastapp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\009_SENAI\02_WhastappSender\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8128D499-2A7B-4094-96D5-5C498E0363F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390035ED-ED94-4C23-A294-CD351384FB83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{7EA62CB6-242D-4E56-A942-578EED957BC9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{7EA62CB6-242D-4E56-A942-578EED957BC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Pessoa</t>
   </si>
@@ -33,34 +33,10 @@
     <t>Número</t>
   </si>
   <si>
-    <t>Mensagem</t>
+    <t>EU</t>
   </si>
   <si>
-    <t>Pessoa 1</t>
-  </si>
-  <si>
-    <t>Pessoa 2</t>
-  </si>
-  <si>
-    <t>Pessoa 3</t>
-  </si>
-  <si>
-    <t>5511999999999</t>
-  </si>
-  <si>
-    <t>5511999999998</t>
-  </si>
-  <si>
-    <t>5511999999997</t>
-  </si>
-  <si>
-    <t>Teste de mensagem 1</t>
-  </si>
-  <si>
-    <t>Teste de mensagem 2</t>
-  </si>
-  <si>
-    <t>Teste de mensagem 3</t>
+    <t>999999999</t>
   </si>
 </sst>
 </file>
@@ -413,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{483B42FD-3844-450C-8A4E-B86FFA35BCA8}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,48 +400,20 @@
     <col min="2" max="2" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Splash Screen e Design de Tela
</commit_message>
<xml_diff>
--- a/ExemploContatosEnviar.xlsx
+++ b/ExemploContatosEnviar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\009_SENAI\02_WhastappSender\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390035ED-ED94-4C23-A294-CD351384FB83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D742547-B0AA-49CD-94D4-616D780A2359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{7EA62CB6-242D-4E56-A942-578EED957BC9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7EA62CB6-242D-4E56-A942-578EED957BC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
     <t>EU</t>
   </si>
   <si>
-    <t>999999999</t>
+    <t>9999999999</t>
   </si>
 </sst>
 </file>
@@ -392,7 +392,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>